<commit_message>
changed eval to support rgbd inputs
</commit_message>
<xml_diff>
--- a/Baseline_summary.xlsx
+++ b/Baseline_summary.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinak\PyCharmsProjects\try\CV_Project-Splatter_Image\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D76540-DF65-48B9-B70D-8D447C7986FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B18C9E-F061-4E94-A2F8-74953BCC32C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{511D045E-1463-4C14-85B5-DFD0A019755E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{511D045E-1463-4C14-85B5-DFD0A019755E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="29">
   <si>
     <t>model1</t>
   </si>
@@ -120,6 +121,9 @@
   </si>
   <si>
     <t>2nd stage time [min]</t>
+  </si>
+  <si>
+    <t>RGBD</t>
   </si>
 </sst>
 </file>
@@ -163,7 +167,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -500,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCB9662-65BF-4657-A953-9C7BF6383DF1}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44:H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -814,7 +818,7 @@
       <c r="E14" s="1">
         <v>-1.9666699999999999</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="1">
         <v>-2.1833100000000001</v>
       </c>
       <c r="G14" s="1">
@@ -840,7 +844,7 @@
       <c r="E15" s="1">
         <v>-1.8955299999999999</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="1">
         <v>-2.1002200000000002</v>
       </c>
       <c r="G15" s="1">
@@ -866,7 +870,7 @@
       <c r="E16" s="1">
         <v>-0.69254000000000004</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="1">
         <v>-0.83923999999999999</v>
       </c>
       <c r="G16" s="1">
@@ -1030,10 +1034,421 @@
       </c>
       <c r="H23" s="1">
         <v>0.25399046462350899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="1">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1">
+        <v>10</v>
+      </c>
+      <c r="D30" s="1">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1">
+        <v>10</v>
+      </c>
+      <c r="G30" s="1">
+        <v>10</v>
+      </c>
+      <c r="H30" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1">
+        <v>64</v>
+      </c>
+      <c r="C31" s="1">
+        <v>64</v>
+      </c>
+      <c r="D31" s="1">
+        <v>64</v>
+      </c>
+      <c r="E31" s="1">
+        <v>64</v>
+      </c>
+      <c r="F31" s="1">
+        <v>64</v>
+      </c>
+      <c r="G31" s="1">
+        <v>64</v>
+      </c>
+      <c r="H31" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="1">
+        <v>128</v>
+      </c>
+      <c r="C32" s="1">
+        <v>128</v>
+      </c>
+      <c r="D32" s="1">
+        <v>64</v>
+      </c>
+      <c r="E32" s="1">
+        <v>64</v>
+      </c>
+      <c r="F32" s="1">
+        <v>64</v>
+      </c>
+      <c r="G32" s="1">
+        <v>64</v>
+      </c>
+      <c r="H32" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>2</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C35" s="1">
+        <v>2500</v>
+      </c>
+      <c r="D35" s="1">
+        <v>4000</v>
+      </c>
+      <c r="E35" s="1">
+        <v>4000</v>
+      </c>
+      <c r="F35" s="1">
+        <v>20000</v>
+      </c>
+      <c r="G35" s="1">
+        <v>4000</v>
+      </c>
+      <c r="H35" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G37" s="1">
+        <v>2000</v>
+      </c>
+      <c r="H37" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="H38" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="1">
+        <v>-1.4129499999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" s="1">
+        <v>-1.3749899999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="1">
+        <v>-0.40711000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" s="1">
+        <v>16.617588993500501</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.74038171056996605</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0.38766978896984999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="1">
+        <v>16.538516728146501</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" s="1">
+        <v>0.72298996468701104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" s="1">
+        <v>0.39756071129966097</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87F2600-C40F-4D16-A365-57F60FE41D1F}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1">
+        <v>24.843500100753499</v>
+      </c>
+      <c r="C2" s="1">
+        <v>16.617588993500501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.93690909885547302</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.74038171056996605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.14556497367183499</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.38766978896984999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>19.529018503075299</v>
+      </c>
+      <c r="C5" s="1">
+        <v>16.538516728146501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.83261579134111996</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.72298996468701104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.25399046462350899</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.39756071129966097</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
run baseline models 3-7 setups on rgbd images created using depth repo
</commit_message>
<xml_diff>
--- a/Baseline_summary.xlsx
+++ b/Baseline_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinak\PyCharmsProjects\try\CV_Project-Splatter_Image\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B18C9E-F061-4E94-A2F8-74953BCC32C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7788646-0730-4B80-B974-136D651A83F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{511D045E-1463-4C14-85B5-DFD0A019755E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
   <si>
     <t>model1</t>
   </si>
@@ -99,9 +99,6 @@
     <t>training_l12_loss</t>
   </si>
   <si>
-    <t>raining_loss</t>
-  </si>
-  <si>
     <t>training_lpips_loss</t>
   </si>
   <si>
@@ -124,6 +121,15 @@
   </si>
   <si>
     <t>RGBD</t>
+  </si>
+  <si>
+    <t>training_loss</t>
+  </si>
+  <si>
+    <t>model7_gaussian_depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -159,15 +165,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -504,10 +507,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCB9662-65BF-4657-A953-9C7BF6383DF1}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44:H49"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -515,8 +521,7 @@
     <col min="1" max="1" width="17.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="11.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.796875" style="1"/>
+    <col min="5" max="8" width="11.8984375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -544,28 +549,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -674,7 +679,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -726,7 +731,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1">
         <v>50</v>
@@ -764,7 +769,7 @@
         <v>2000</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1">
         <v>10000</v>
@@ -778,7 +783,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1">
         <v>180</v>
@@ -790,7 +795,7 @@
         <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1">
         <v>105</v>
@@ -815,8 +820,8 @@
       <c r="D14" s="1">
         <v>-1.9666697677095</v>
       </c>
-      <c r="E14" s="1">
-        <v>-1.9666699999999999</v>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="F14" s="1">
         <v>-2.1833100000000001</v>
@@ -830,7 +835,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1">
         <v>-1.72549</v>
@@ -842,7 +847,7 @@
         <v>-1.89552819209829</v>
       </c>
       <c r="E15" s="1">
-        <v>-1.8955299999999999</v>
+        <v>-2.0053948592137401</v>
       </c>
       <c r="F15" s="1">
         <v>-2.1002200000000002</v>
@@ -856,7 +861,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>-0.64695000000000003</v>
@@ -867,8 +872,8 @@
       <c r="D16" s="1">
         <v>-0.69253510035399302</v>
       </c>
-      <c r="E16" s="1">
-        <v>-0.69254000000000004</v>
+      <c r="E16" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="F16" s="1">
         <v>-0.83923999999999999</v>
@@ -880,7 +885,7 @@
         <v>-0.66279999999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -906,7 +911,7 @@
         <v>24.843500100753499</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -932,7 +937,7 @@
         <v>0.93690909885547302</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -958,7 +963,7 @@
         <v>0.14556497367183499</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -984,7 +989,7 @@
         <v>19.529018503075299</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1010,7 +1015,7 @@
         <v>0.83261579134111996</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1036,7 +1041,7 @@
         <v>0.25399046462350899</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
@@ -1058,34 +1063,40 @@
       <c r="H27" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J27" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1110,8 +1121,11 @@
       <c r="H29" s="2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J29" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -1136,8 +1150,11 @@
       <c r="H30" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J30" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1162,8 +1179,11 @@
       <c r="H31" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J31" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1188,10 +1208,13 @@
       <c r="H32" s="1">
         <v>64</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J32" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
@@ -1214,8 +1237,15 @@
       <c r="H33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H34"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1240,16 +1270,34 @@
       <c r="H35" s="1">
         <v>4000</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J35" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="1">
+        <v>60</v>
+      </c>
+      <c r="E36" s="1">
+        <v>173</v>
+      </c>
+      <c r="F36" s="1">
+        <v>207</v>
+      </c>
+      <c r="G36" s="1">
         <v>26</v>
       </c>
-      <c r="H36" s="3">
+      <c r="H36" s="1">
+        <v>43</v>
+      </c>
+      <c r="J36" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1263,7 +1311,7 @@
         <v>2000</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F37" s="1">
         <v>10000</v>
@@ -1274,85 +1322,250 @@
       <c r="H37" s="1">
         <v>2000</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J37" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="1">
+        <v>39</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="1">
+        <v>139</v>
+      </c>
+      <c r="G38" s="1">
+        <v>18</v>
+      </c>
+      <c r="H38" s="1">
         <v>27</v>
       </c>
-      <c r="H38" s="1">
+      <c r="J38" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H39"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
+      <c r="D40" s="1">
+        <v>-1.9505999999999999</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="1">
+        <v>-2.1755900000000001</v>
+      </c>
+      <c r="G40" s="1">
+        <v>-1.97624</v>
+      </c>
       <c r="H40" s="1">
+        <v>-2.0394600000000001</v>
+      </c>
+      <c r="J40" s="1">
         <v>-1.4129499999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" s="1">
+        <v>-1.88059</v>
+      </c>
+      <c r="E41" s="1">
+        <v>-2.0607899999999999</v>
+      </c>
+      <c r="F41" s="1">
+        <v>-2.0973999999999999</v>
+      </c>
+      <c r="G41" s="1">
+        <v>-1.90368</v>
+      </c>
+      <c r="H41" s="1">
+        <v>-1.9544600000000001</v>
+      </c>
+      <c r="J41" s="1">
+        <v>-1.3749899999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>20</v>
       </c>
-      <c r="H41" s="1">
-        <v>-1.3749899999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>21</v>
+      <c r="D42" s="1">
+        <v>-0.68359999999999999</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="1">
+        <v>-0.85907</v>
+      </c>
+      <c r="G42" s="1">
+        <v>-0.69328999999999996</v>
       </c>
       <c r="H42" s="1">
+        <v>-0.68501999999999996</v>
+      </c>
+      <c r="J42" s="1">
         <v>-0.40711000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>13</v>
       </c>
+      <c r="D44" s="1">
+        <v>24.389944022352001</v>
+      </c>
+      <c r="E44" s="1">
+        <v>22.9174979522146</v>
+      </c>
+      <c r="F44" s="1">
+        <v>27.853587666018399</v>
+      </c>
+      <c r="G44" s="1">
+        <v>24.4577316045761</v>
+      </c>
       <c r="H44" s="1">
+        <v>24.568996774879299</v>
+      </c>
+      <c r="J44" s="1">
         <v>16.617588993500501</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>14</v>
       </c>
+      <c r="D45" s="1">
+        <v>0.93189543384042595</v>
+      </c>
+      <c r="E45" s="1">
+        <v>0.91504740897058001</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0.96756165754050005</v>
+      </c>
+      <c r="G45" s="1">
+        <v>0.93258147111960799</v>
+      </c>
       <c r="H45" s="1">
+        <v>0.93394670195200202</v>
+      </c>
+      <c r="J45" s="1">
         <v>0.74038171056996605</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>15</v>
       </c>
+      <c r="D46" s="1">
+        <v>0.155842035871253</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0.18676805534844501</v>
+      </c>
+      <c r="F46" s="1">
+        <v>7.5002662910264903E-2</v>
+      </c>
+      <c r="G46" s="1">
+        <v>0.153533073301826</v>
+      </c>
       <c r="H46" s="1">
+        <v>0.15085613816468499</v>
+      </c>
+      <c r="J46" s="1">
         <v>0.38766978896984999</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>16</v>
       </c>
+      <c r="D47" s="1">
+        <v>19.4644615606726</v>
+      </c>
+      <c r="E47" s="1">
+        <v>20.851605018534801</v>
+      </c>
+      <c r="F47" s="1">
+        <v>21.020306886796899</v>
+      </c>
+      <c r="G47" s="1">
+        <v>19.317035862513901</v>
+      </c>
       <c r="H47" s="1">
+        <v>19.4829776251654</v>
+      </c>
+      <c r="J47" s="1">
         <v>16.538516728146501</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>17</v>
       </c>
+      <c r="D48" s="1">
+        <v>0.83611995374411197</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0.862037195321532</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0.86831759352372495</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0.83297753747871905</v>
+      </c>
       <c r="H48" s="1">
+        <v>0.83742460306056499</v>
+      </c>
+      <c r="J48" s="1">
         <v>0.72298996468701104</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>18</v>
       </c>
+      <c r="D49" s="1">
+        <v>0.25300177754326297</v>
+      </c>
+      <c r="E49" s="1">
+        <v>0.24988846171387299</v>
+      </c>
+      <c r="F49" s="1">
+        <v>0.190097852033623</v>
+      </c>
+      <c r="G49" s="1">
+        <v>0.25675172067241903</v>
+      </c>
       <c r="H49" s="1">
+        <v>0.249459170793945</v>
+      </c>
+      <c r="J49" s="1">
         <v>0.39756071129966097</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G51" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1376,10 +1589,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated comparison to baseline results to be more readable
</commit_message>
<xml_diff>
--- a/Baseline_summary.xlsx
+++ b/Baseline_summary.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinak\PyCharmsProjects\try\CV_Project-Splatter_Image\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71932BFD-EA62-4B41-9564-E060AC3138BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA483F30-BD89-41FF-B9FF-3132877BBCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{511D045E-1463-4C14-85B5-DFD0A019755E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{511D045E-1463-4C14-85B5-DFD0A019755E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="co3d" sheetId="2" r:id="rId2"/>
-    <sheet name="splatter_image" sheetId="3" r:id="rId3"/>
+    <sheet name="srn_cars_100%" sheetId="4" r:id="rId2"/>
+    <sheet name="srn_cars_50%" sheetId="5" r:id="rId3"/>
+    <sheet name="srn_cars_20%" sheetId="6" r:id="rId4"/>
+    <sheet name="co3d_w_background" sheetId="2" r:id="rId5"/>
+    <sheet name="co3d_wo_background" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,13 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="36">
-  <si>
-    <t>model1</t>
-  </si>
-  <si>
-    <t>model2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="43">
   <si>
     <t>model3</t>
   </si>
@@ -145,7 +142,34 @@
     <t>C:\Users\dinak\PyCharmsProjects\try\CV_Project-Splatter_Image\experiments_out\2024-10-09\20-19-54</t>
   </si>
   <si>
-    <t>RGB_WB</t>
+    <t>C:\Users\dinak\PyCharmsProjects\try\CV_Project-Splatter_Image\experiments_out\cars_co3d_rgb_100%_20000_2000_w_back\01-52-01</t>
+  </si>
+  <si>
+    <t>C:\Users\dinak\PyCharmsProjects\try\CV_Project-Splatter_Image\experiments_out\cars_co3d_rgb_100%_20000_2000_w_back\07-53-08</t>
+  </si>
+  <si>
+    <t>srn_cars</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>RGBD_SI</t>
+  </si>
+  <si>
+    <t>RGBD_NN</t>
+  </si>
+  <si>
+    <t>RGBD_NN_OUT_DEPTH</t>
+  </si>
+  <si>
+    <t>cars_co3d with background</t>
+  </si>
+  <si>
+    <t>cars_co3d without background</t>
+  </si>
+  <si>
+    <t>RGBD_SI_OUT_DEPTH</t>
   </si>
 </sst>
 </file>
@@ -161,12 +185,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -181,13 +211,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,10 +563,10 @@
   <dimension ref="A1:M99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E68" sqref="E68"/>
+      <selection pane="bottomRight" activeCell="E90" sqref="E90:E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -541,44 +578,44 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -598,7 +635,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>10</v>
@@ -618,7 +655,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>64</v>
@@ -638,7 +675,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>64</v>
@@ -658,7 +695,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -678,9 +715,9 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
         <v>4000</v>
       </c>
       <c r="C9" s="1">
@@ -689,18 +726,18 @@
       <c r="D9" s="1">
         <v>20000</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="3">
         <v>4000</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>4000</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="1">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3">
         <v>40</v>
       </c>
       <c r="C10" s="1">
@@ -709,78 +746,83 @@
       <c r="D10" s="1">
         <v>165</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <v>25</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3">
         <v>2000</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1">
         <v>10000</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="3">
         <v>2000</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <v>2000</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="1">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3">
         <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" s="1">
         <v>105</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <v>18</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <v>23</v>
       </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="1">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3">
         <v>-1.9666697677095</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1">
         <v>-2.1833100000000001</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="3">
         <v>-2.0167199999999998</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="3">
         <v>-1.9105099999999999</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="1">
+        <v>26</v>
+      </c>
+      <c r="B15" s="3">
         <v>-1.89552819209829</v>
       </c>
       <c r="C15" s="1">
@@ -789,38 +831,43 @@
       <c r="D15" s="1">
         <v>-2.1002200000000002</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="3">
         <v>-1.93493</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="3">
         <v>-1.84348</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="1">
+        <v>18</v>
+      </c>
+      <c r="B16" s="3">
         <v>-0.69253510035399302</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D16" s="1">
         <v>-0.83923999999999999</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="3">
         <v>-0.67979999999999996</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="3">
         <v>-0.66279999999999994</v>
       </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
+        <v>11</v>
+      </c>
+      <c r="B18" s="3">
         <v>24.5525351522321</v>
       </c>
       <c r="C18" s="1">
@@ -829,18 +876,18 @@
       <c r="D18" s="1">
         <v>28.082735555415798</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="3">
         <v>24.595531480652902</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="3">
         <v>24.843500100753499</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="1">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3">
         <v>0.93258934129368098</v>
       </c>
       <c r="C19" s="1">
@@ -849,18 +896,18 @@
       <c r="D19" s="1">
         <v>0.96839865737340602</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="3">
         <v>0.93330415189266203</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="3">
         <v>0.93690909885547302</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="1">
+        <v>13</v>
+      </c>
+      <c r="B20" s="3">
         <v>0.15133590520020901</v>
       </c>
       <c r="C20" s="1">
@@ -869,18 +916,18 @@
       <c r="D20" s="1">
         <v>8.5103769272708699E-2</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="3">
         <v>0.15459601692855299</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="3">
         <v>0.14556497367183499</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="1">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3">
         <v>19.556921948736299</v>
       </c>
       <c r="C21" s="1">
@@ -889,18 +936,18 @@
       <c r="D21" s="1">
         <v>20.966884533925398</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="3">
         <v>19.308173245702399</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="3">
         <v>19.529018503075299</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="1">
+        <v>15</v>
+      </c>
+      <c r="B22" s="3">
         <v>0.83340076460011903</v>
       </c>
       <c r="C22" s="1">
@@ -909,18 +956,18 @@
       <c r="D22" s="1">
         <v>0.86850320007855197</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="3">
         <v>0.82982315452780098</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="3">
         <v>0.83261579134111996</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="1">
+        <v>16</v>
+      </c>
+      <c r="B23" s="3">
         <v>0.25596143542445998</v>
       </c>
       <c r="C23" s="1">
@@ -929,53 +976,53 @@
       <c r="D23" s="1">
         <v>0.19304196769913801</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="3">
         <v>0.25545847610831202</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="3">
         <v>0.25399046462350899</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
@@ -995,7 +1042,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B30" s="1">
         <v>10</v>
@@ -1015,7 +1062,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B31" s="1">
         <v>64</v>
@@ -1035,7 +1082,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1">
         <v>64</v>
@@ -1055,7 +1102,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
@@ -1078,9 +1125,9 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="1">
+        <v>8</v>
+      </c>
+      <c r="B35" s="3">
         <v>4000</v>
       </c>
       <c r="C35" s="1">
@@ -1089,18 +1136,18 @@
       <c r="D35" s="1">
         <v>20000</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="3">
         <v>4000</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="3">
         <v>4000</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="1">
+        <v>23</v>
+      </c>
+      <c r="B36" s="3">
         <v>60</v>
       </c>
       <c r="C36" s="1">
@@ -1109,81 +1156,83 @@
       <c r="D36" s="1">
         <v>207</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="3">
         <v>26</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="3">
         <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="1">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3">
         <v>2000</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D37" s="1">
         <v>10000</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="3">
         <v>2000</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="3">
         <v>2000</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="1">
+        <v>24</v>
+      </c>
+      <c r="B38" s="3">
         <v>39</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D38" s="1">
         <v>139</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="3">
         <v>18</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="3">
         <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F39"/>
+      <c r="B39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="1">
+        <v>17</v>
+      </c>
+      <c r="B40" s="3">
         <v>-1.9505999999999999</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D40" s="1">
         <v>-2.1755900000000001</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="3">
         <v>-1.97624</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="3">
         <v>-2.0394600000000001</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41" s="1">
+        <v>26</v>
+      </c>
+      <c r="B41" s="3">
         <v>-1.88059</v>
       </c>
       <c r="C41" s="1">
@@ -1192,10 +1241,10 @@
       <c r="D41" s="1">
         <v>-2.0973999999999999</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="3">
         <v>-1.90368</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="3">
         <v>-1.9544600000000001</v>
       </c>
       <c r="I41">
@@ -1221,21 +1270,21 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" s="1">
+        <v>18</v>
+      </c>
+      <c r="B42" s="3">
         <v>-0.68359999999999999</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D42" s="1">
         <v>-0.85907</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="3">
         <v>-0.69328999999999996</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="3">
         <v>-0.68501999999999996</v>
       </c>
       <c r="I42">
@@ -1260,6 +1309,9 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
       <c r="I43">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1283,9 +1335,9 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" s="1">
+        <v>11</v>
+      </c>
+      <c r="B44" s="3">
         <v>24.389944022352001</v>
       </c>
       <c r="C44" s="1">
@@ -1294,38 +1346,38 @@
       <c r="D44" s="1">
         <v>27.853587666018399</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="3">
         <v>24.4577316045761</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="3">
         <v>24.568996774879299</v>
       </c>
       <c r="I44">
-        <f>IF(B47&gt;B21,1,0)</f>
+        <f t="shared" ref="I44:M45" si="3">IF(B47&gt;B21,1,0)</f>
         <v>0</v>
       </c>
       <c r="J44">
-        <f>IF(C47&gt;C21,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K44">
-        <f>IF(D47&gt;D21,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L44">
-        <f>IF(E47&gt;E21,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M44">
-        <f>IF(F47&gt;F21,1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="1">
+        <v>12</v>
+      </c>
+      <c r="B45" s="3">
         <v>0.93189543384042595</v>
       </c>
       <c r="C45" s="1">
@@ -1334,38 +1386,38 @@
       <c r="D45" s="1">
         <v>0.96756165754050005</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="3">
         <v>0.93258147111960799</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="3">
         <v>0.93394670195200202</v>
       </c>
       <c r="I45">
-        <f>IF(B48&gt;B22,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J45">
-        <f>IF(C48&gt;C22,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K45">
-        <f>IF(D48&gt;D22,1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L45">
-        <f>IF(E48&gt;E22,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M45">
-        <f>IF(F48&gt;F22,1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>15</v>
-      </c>
-      <c r="B46" s="1">
+        <v>13</v>
+      </c>
+      <c r="B46" s="3">
         <v>0.155842035871253</v>
       </c>
       <c r="C46" s="1">
@@ -1374,10 +1426,10 @@
       <c r="D46" s="1">
         <v>7.5002662910264903E-2</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="3">
         <v>0.153533073301826</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46" s="3">
         <v>0.15085613816468499</v>
       </c>
       <c r="I46">
@@ -1385,27 +1437,27 @@
         <v>1</v>
       </c>
       <c r="J46">
-        <f t="shared" ref="J46:M46" si="3">IF(C49&lt;C23,1,0)</f>
+        <f t="shared" ref="J46:M46" si="4">IF(C49&lt;C23,1,0)</f>
         <v>0</v>
       </c>
       <c r="K46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="1">
+        <v>14</v>
+      </c>
+      <c r="B47" s="3">
         <v>19.4644615606726</v>
       </c>
       <c r="C47" s="1">
@@ -1414,18 +1466,18 @@
       <c r="D47" s="1">
         <v>21.020306886796899</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="3">
         <v>19.317035862513901</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47" s="3">
         <v>19.4829776251654</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>17</v>
-      </c>
-      <c r="B48" s="1">
+        <v>15</v>
+      </c>
+      <c r="B48" s="3">
         <v>0.83611995374411197</v>
       </c>
       <c r="C48" s="1">
@@ -1434,18 +1486,18 @@
       <c r="D48" s="1">
         <v>0.86831759352372495</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="3">
         <v>0.83297753747871905</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48" s="3">
         <v>0.83742460306056499</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>18</v>
-      </c>
-      <c r="B49" s="1">
+        <v>16</v>
+      </c>
+      <c r="B49" s="3">
         <v>0.25300177754326297</v>
       </c>
       <c r="C49" s="1">
@@ -1454,53 +1506,53 @@
       <c r="D49" s="1">
         <v>0.190097852033623</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="3">
         <v>0.25675172067241903</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F49" s="3">
         <v>0.249459170793945</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E52" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B54" s="2">
         <v>1</v>
@@ -1520,7 +1572,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B55" s="1">
         <v>10</v>
@@ -1540,7 +1592,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B56" s="1">
         <v>64</v>
@@ -1560,7 +1612,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B57" s="1">
         <v>64</v>
@@ -1580,7 +1632,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B58" s="1">
         <v>1</v>
@@ -1600,9 +1652,9 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>10</v>
-      </c>
-      <c r="B60" s="1">
+        <v>8</v>
+      </c>
+      <c r="B60" s="3">
         <v>4000</v>
       </c>
       <c r="C60" s="1">
@@ -1611,233 +1663,240 @@
       <c r="D60" s="1">
         <v>20000</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="3">
         <v>4000</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F60" s="3">
         <v>4000</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>25</v>
-      </c>
-      <c r="B61" s="1">
+        <v>23</v>
+      </c>
+      <c r="B61" s="3">
         <v>46</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61" s="3">
         <v>61</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="3">
         <v>36</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>9</v>
-      </c>
-      <c r="B62" s="1">
+        <v>7</v>
+      </c>
+      <c r="B62" s="3">
         <v>2000</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D62" s="1">
         <v>10000</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="3">
         <v>2000</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62" s="3">
         <v>2000</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="3">
+        <v>36</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63" s="3">
+        <v>35</v>
+      </c>
+      <c r="F63" s="3">
         <v>26</v>
       </c>
-      <c r="B63" s="1">
-        <v>36</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E63" s="1">
-        <v>35</v>
-      </c>
-      <c r="F63" s="1">
-        <v>26</v>
-      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F64"/>
+      <c r="B64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="4"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>19</v>
-      </c>
-      <c r="B65" s="1">
+        <v>17</v>
+      </c>
+      <c r="B65" s="3">
         <v>-1.92777</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="3">
         <v>-1.96295</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65" s="3">
         <v>-1.99211</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>28</v>
-      </c>
-      <c r="B66" s="1">
+        <v>26</v>
+      </c>
+      <c r="B66" s="3">
         <v>-1.86063</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66" s="3">
         <v>-1.8900699999999999</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F66" s="3">
         <v>-1.91327</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>20</v>
-      </c>
-      <c r="B67" s="1">
+        <v>18</v>
+      </c>
+      <c r="B67" s="3">
         <v>-0.67934000000000005</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67" s="3">
         <v>-0.67803999999999998</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F67" s="3">
         <v>-0.67184999999999995</v>
       </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>13</v>
-      </c>
-      <c r="B69" s="1">
+        <v>11</v>
+      </c>
+      <c r="B69" s="3">
         <v>24.716734161431098</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69" s="3">
         <v>24.678975658757299</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F69" s="3">
         <v>24.776949598030601</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>14</v>
-      </c>
-      <c r="B70" s="1">
+        <v>12</v>
+      </c>
+      <c r="B70" s="3">
         <v>0.93650351981209001</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70" s="3">
         <v>0.93395875309194798</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F70" s="3">
         <v>0.93665950592945901</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>15</v>
-      </c>
-      <c r="B71" s="1">
+        <v>13</v>
+      </c>
+      <c r="B71" s="3">
         <v>0.15061360494953299</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71" s="3">
         <v>0.154813281074166</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F71" s="3">
         <v>0.14911564117805501</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>16</v>
-      </c>
-      <c r="B72" s="1">
+        <v>14</v>
+      </c>
+      <c r="B72" s="3">
         <v>18.931579110131299</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="3">
         <v>18.725503152489601</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F72" s="3">
         <v>18.974213619055998</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>17</v>
-      </c>
-      <c r="B73" s="1">
+        <v>15</v>
+      </c>
+      <c r="B73" s="3">
         <v>0.824433115605264</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73" s="3">
         <v>0.81939109509672403</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F73" s="3">
         <v>0.82252721977640197</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>18</v>
-      </c>
-      <c r="B74" s="1">
+        <v>16</v>
+      </c>
+      <c r="B74" s="3">
         <v>0.26398986027508298</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74" s="3">
         <v>0.26631626155525401</v>
       </c>
-      <c r="F74" s="1">
+      <c r="F74" s="3">
         <v>0.26509950286700301</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E77" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B79" s="2">
         <v>1</v>
@@ -1857,7 +1916,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B80" s="1">
         <v>10</v>
@@ -1877,7 +1936,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B81" s="1">
         <v>64</v>
@@ -1897,7 +1956,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B82" s="1">
         <v>64</v>
@@ -1917,7 +1976,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B83" s="1">
         <v>1</v>
@@ -1937,7 +1996,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B85" s="1">
         <v>4000</v>
@@ -1957,7 +2016,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E86" s="1">
         <v>58</v>
@@ -1965,13 +2024,13 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B87" s="1">
         <v>2000</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D87" s="1">
         <v>10000</v>
@@ -1985,10 +2044,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E88" s="1">
         <v>34</v>
@@ -1999,56 +2058,47 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>19</v>
-      </c>
-      <c r="E90" s="1">
-        <v>-1.42222</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>28</v>
-      </c>
-      <c r="E91" s="1">
-        <v>-1.3843300000000001</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>20</v>
-      </c>
-      <c r="E92" s="1">
-        <v>-0.41722999999999999</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2058,11 +2108,797 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87F2600-C40F-4D16-A365-57F60FE41D1F}">
-  <dimension ref="A1:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B34FC15-96D8-4303-9AB1-880B3B105DEB}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-1.9666697677095</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-1.92777</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-1.9505999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-1.89552819209829</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-1.86063</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-1.88059</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.69253510035399302</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-0.67934000000000005</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-0.68359999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>24.5525351522321</v>
+      </c>
+      <c r="C16" s="1">
+        <v>24.716734161431098</v>
+      </c>
+      <c r="D16" s="1">
+        <v>24.389944022352001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.93258934129368098</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.93650351981209001</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.93189543384042595</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.15133590520020901</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.15061360494953299</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.155842035871253</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>19.556921948736299</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18.931579110131299</v>
+      </c>
+      <c r="D19" s="1">
+        <v>19.4644615606726</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.83340076460011903</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.824433115605264</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.83611995374411197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.25596143542445998</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.26398986027508298</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.25300177754326297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>40</v>
+      </c>
+      <c r="C23" s="1">
+        <v>46</v>
+      </c>
+      <c r="D23" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1">
+        <v>36</v>
+      </c>
+      <c r="D24" s="1">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72949DC4-D34C-4434-B271-9E5CE6E9CA21}">
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-1.9105099999999999</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-1.99211</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-2.0394600000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-1.84348</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-1.91327</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-1.9544600000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.66279999999999994</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-0.67184999999999995</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-0.68501999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>24.843500100753499</v>
+      </c>
+      <c r="C16" s="1">
+        <v>24.776949598030601</v>
+      </c>
+      <c r="D16" s="1">
+        <v>24.568996774879299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.93690909885547302</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.93665950592945901</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.93394670195200202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.14556497367183499</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.14911564117805501</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.15085613816468499</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>19.529018503075299</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18.974213619055998</v>
+      </c>
+      <c r="D19" s="1">
+        <v>19.4829776251654</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.83261579134111996</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.82252721977640197</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.83742460306056499</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.25399046462350899</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.26509950286700301</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.249459170793945</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1">
+        <v>26</v>
+      </c>
+      <c r="D24" s="1">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B20978-D809-4F22-B392-B7FE2B5D1F45}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-2.0167199999999998</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-1.96295</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-1.97624</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-1.93493</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-1.8900699999999999</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-1.90368</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.67979999999999996</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-0.67803999999999998</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-0.69328999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>24.595531480652902</v>
+      </c>
+      <c r="C16" s="1">
+        <v>24.678975658757299</v>
+      </c>
+      <c r="D16" s="1">
+        <v>24.4577316045761</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.93330415189266203</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.93395875309194798</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.93258147111960799</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.15459601692855299</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.154813281074166</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.153533073301826</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>19.308173245702399</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18.725503152489601</v>
+      </c>
+      <c r="D19" s="1">
+        <v>19.317035862513901</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.82982315452780098</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.81939109509672403</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.83297753747871905</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.25545847610831202</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.26631626155525401</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.25675172067241903</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1">
+        <v>61</v>
+      </c>
+      <c r="D23" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1">
+        <v>35</v>
+      </c>
+      <c r="D24" s="1">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87F2600-C40F-4D16-A365-57F60FE41D1F}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2070,298 +2906,239 @@
     <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>128</v>
       </c>
-      <c r="C5" s="1">
-        <v>128</v>
-      </c>
-      <c r="D5" s="1">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>64</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1">
-        <v>64</v>
-      </c>
-      <c r="C6" s="1">
-        <v>64</v>
-      </c>
-      <c r="D6" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" s="1">
+        <v>20000</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>20000</v>
-      </c>
-      <c r="C9" s="1">
-        <v>20000</v>
-      </c>
-      <c r="D9" s="1">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="1">
-        <v>225</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1">
-        <v>2000</v>
+        <v>-1.45949</v>
       </c>
       <c r="C12" s="1">
-        <v>2000</v>
-      </c>
-      <c r="D12" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-1.36934</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="1">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-1.39194</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-1.3091600000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.20835000000000001</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-0.16894999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1">
-        <v>-1.4845600000000001</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1">
-        <v>-1.36934</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22.1906239986419</v>
+      </c>
+      <c r="C16" s="1">
+        <v>21.0609602332115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1">
-        <v>-1.4308799999999999</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1">
-        <v>-1.3091600000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.71046415865421297</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.64678486585617001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1">
-        <v>-0.33359</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1">
-        <v>-0.16894999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.39445140957832298</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.48273735195398298</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>14.001488065138</v>
+      </c>
+      <c r="C19" s="1">
+        <v>13.9242058409802</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1">
-        <v>27.3742079734802</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1">
-        <v>21.0609602332115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.38057947905823297</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.37298560538075598</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1">
-        <v>0.92927645742893195</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1">
-        <v>0.64678486585617001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.13171484395861599</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1">
-        <v>0.48273735195398298</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.67616527564101303</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.68830526059604002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
-        <v>16.589788734894899</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1">
-        <v>13.9242058409802</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="C23" s="1">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
-        <v>0.54950548779116803</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1">
-        <v>0.37298560538075598</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0.42677373654784101</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1">
-        <v>0.68830526059604002</v>
+        <v>22</v>
+      </c>
+      <c r="C24" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2369,39 +3146,200 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C86E3A39-9A6F-4CA1-8C84-8B0851F3DB1B}">
-  <dimension ref="B2:C7"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FC7724-FE73-4AF6-9A61-4A0445399B4C}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.19921875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-1.4845600000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-1.4308799999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.33359</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>27.3742079734802</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.92927645742893195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.13171484395861599</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>16.589788734894899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.54950548779116803</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.42677373654784101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated 100% data results
</commit_message>
<xml_diff>
--- a/Baseline_summary.xlsx
+++ b/Baseline_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinak\PyCharmsProjects\try\CV_Project-Splatter_Image\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA483F30-BD89-41FF-B9FF-3132877BBCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4349D566-F7BA-47D5-9011-95CD70314A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{511D045E-1463-4C14-85B5-DFD0A019755E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{511D045E-1463-4C14-85B5-DFD0A019755E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,10 +176,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,6 +241,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,10 +585,10 @@
   <dimension ref="A1:M99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E90" sqref="E90:E92"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2111,8 +2133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B34FC15-96D8-4303-9AB1-880B3B105DEB}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2220,6 +2242,12 @@
       <c r="D12" s="1">
         <v>-1.9505999999999999</v>
       </c>
+      <c r="E12" s="1">
+        <v>-1.9135</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-1.9183300000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2234,6 +2262,12 @@
       <c r="D13" s="1">
         <v>-1.88059</v>
       </c>
+      <c r="E13" s="1">
+        <v>-1.84918</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-1.85304</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2247,12 +2281,20 @@
       </c>
       <c r="D14" s="1">
         <v>-0.68359999999999999</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-0.68400000000000005</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-0.68225000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2267,8 +2309,14 @@
       <c r="D16" s="1">
         <v>24.389944022352001</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <v>24.737295589663699</v>
+      </c>
+      <c r="F16" s="1">
+        <v>24.7535391118038</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2281,8 +2329,14 @@
       <c r="D17" s="1">
         <v>0.93189543384042595</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>0.93629159058698197</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.93711998567662402</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2295,12 +2349,18 @@
       <c r="D18" s="1">
         <v>0.155842035871253</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1">
+        <v>0.15091960154346701</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.14831589974081899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="7">
         <v>19.556921948736299</v>
       </c>
       <c r="C19" s="1">
@@ -2309,8 +2369,14 @@
       <c r="D19" s="1">
         <v>19.4644615606726</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1">
+        <v>18.8896101027761</v>
+      </c>
+      <c r="F19" s="1">
+        <v>18.946477096588701</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2320,11 +2386,17 @@
       <c r="C20" s="1">
         <v>0.824433115605264</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="7">
         <v>0.83611995374411197</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1">
+        <v>0.82427795599265596</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.82487530109726404</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2334,11 +2406,20 @@
       <c r="C21" s="1">
         <v>0.26398986027508298</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="7">
         <v>0.25300177754326297</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="1">
+        <v>0.26353628302848098</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.26368653031844902</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2351,8 +2432,14 @@
       <c r="D23" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1">
+        <v>60</v>
+      </c>
+      <c r="F23" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2364,6 +2451,12 @@
       </c>
       <c r="D24" s="1">
         <v>39</v>
+      </c>
+      <c r="E24" s="1">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2373,10 +2466,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72949DC4-D34C-4434-B271-9E5CE6E9CA21}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2529,7 +2622,7 @@
         <v>24.568996774879299</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2543,7 +2636,7 @@
         <v>0.93394670195200202</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2557,11 +2650,11 @@
         <v>0.15085613816468499</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="6">
         <v>19.529018503075299</v>
       </c>
       <c r="C19" s="1">
@@ -2570,8 +2663,12 @@
       <c r="D19" s="1">
         <v>19.4829776251654</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f>MAX(B19:F19)</f>
+        <v>19.529018503075299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2581,11 +2678,15 @@
       <c r="C20" s="1">
         <v>0.82252721977640197</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="6">
         <v>0.83742460306056499</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f>MAX(B20:F20)</f>
+        <v>0.83742460306056499</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2595,11 +2696,15 @@
       <c r="C21" s="1">
         <v>0.26509950286700301</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="6">
         <v>0.249459170793945</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f>MIN(B21:F21)</f>
+        <v>0.249459170793945</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2613,7 +2718,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2637,7 +2742,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2828,7 +2933,7 @@
       <c r="C19" s="1">
         <v>18.725503152489601</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="6">
         <v>19.317035862513901</v>
       </c>
     </row>
@@ -2842,7 +2947,7 @@
       <c r="C20" s="1">
         <v>0.81939109509672403</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="6">
         <v>0.83297753747871905</v>
       </c>
     </row>
@@ -2850,7 +2955,7 @@
       <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="6">
         <v>0.25545847610831202</v>
       </c>
       <c r="C21" s="1">
@@ -2895,10 +3000,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87F2600-C40F-4D16-A365-57F60FE41D1F}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3042,7 +3147,7 @@
         <v>21.0609602332115</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3053,7 +3158,7 @@
         <v>0.64678486585617001</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -3064,40 +3169,52 @@
         <v>0.48273735195398298</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="6">
         <v>14.001488065138</v>
       </c>
       <c r="C19" s="1">
         <v>13.9242058409802</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f>MAX(B19:C19)</f>
+        <v>14.001488065138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="6">
         <v>0.38057947905823297</v>
       </c>
       <c r="C20" s="1">
         <v>0.37298560538075598</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f t="shared" ref="I20:I21" si="0">MAX(B20:C20)</f>
+        <v>0.38057947905823297</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="6">
         <v>0.67616527564101303</v>
       </c>
       <c r="C21" s="1">
         <v>0.68830526059604002</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f>MIN(B21:C21)</f>
+        <v>0.67616527564101303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3108,7 +3225,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3119,7 +3236,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -3130,7 +3247,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
fixed issue related to replacing the output depth with the input channel depth
</commit_message>
<xml_diff>
--- a/Baseline_summary.xlsx
+++ b/Baseline_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinak\PyCharmsProjects\try\CV_Project-Splatter_Image\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DBF3F3-7141-484E-8900-FCC4062F7295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5290103C-236E-49A7-91CB-39F9FCF0B027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{511D045E-1463-4C14-85B5-DFD0A019755E}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="43">
   <si>
     <t>model3</t>
   </si>
@@ -2698,7 +2698,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2786,9 +2786,6 @@
       <c r="E11" t="s">
         <v>42</v>
       </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2803,10 +2800,10 @@
       <c r="D12" s="1">
         <v>-1.97624</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1">
-        <v>-1.56101</v>
-      </c>
+      <c r="E12" s="1">
+        <v>-1.67428</v>
+      </c>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2821,10 +2818,10 @@
       <c r="D13" s="1">
         <v>-1.90368</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1">
-        <v>-1.51372</v>
-      </c>
+      <c r="E13" s="1">
+        <v>-1.61931</v>
+      </c>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2839,10 +2836,10 @@
       <c r="D14" s="1">
         <v>-0.69328999999999996</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
-        <v>-0.46400000000000002</v>
-      </c>
+      <c r="E14" s="1">
+        <v>-0.51312999999999998</v>
+      </c>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
@@ -2864,10 +2861,10 @@
       <c r="D16" s="1">
         <v>24.4577316045761</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
-        <v>16.8412933264459</v>
-      </c>
+      <c r="E16" s="1">
+        <v>14.9439022881644</v>
+      </c>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2882,10 +2879,10 @@
       <c r="D17" s="1">
         <v>0.93258147111960799</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1">
-        <v>0.75915334011827196</v>
-      </c>
+      <c r="E17" s="1">
+        <v>0.73801240793296197</v>
+      </c>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -2900,10 +2897,10 @@
       <c r="D18" s="1">
         <v>0.153533073301826</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1">
-        <v>0.39463289912257798</v>
-      </c>
+      <c r="E18" s="1">
+        <v>0.32750347650476802</v>
+      </c>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -2918,10 +2915,10 @@
       <c r="D19" s="6">
         <v>19.317035862513901</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1">
-        <v>13.884638862916299</v>
-      </c>
+      <c r="E19" s="1">
+        <v>13.3197594721317</v>
+      </c>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2936,10 +2933,10 @@
       <c r="D20" s="6">
         <v>0.83297753747871905</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1">
-        <v>0.62399948857852405</v>
-      </c>
+      <c r="E20" s="1">
+        <v>0.64797816423518295</v>
+      </c>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2954,10 +2951,10 @@
       <c r="D21" s="1">
         <v>0.25675172067241903</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1">
-        <v>0.49321661506593201</v>
-      </c>
+      <c r="E21" s="1">
+        <v>0.39727669408959898</v>
+      </c>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E22" s="1"/>
@@ -2979,9 +2976,7 @@
       <c r="E23" s="1">
         <v>60</v>
       </c>
-      <c r="F23" s="1">
-        <v>66</v>
-      </c>
+      <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -2996,10 +2991,10 @@
       <c r="D24" s="1">
         <v>18</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1">
-        <v>18</v>
-      </c>
+      <c r="E24" s="1">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cleaned project and added project summary
</commit_message>
<xml_diff>
--- a/Baseline_summary.xlsx
+++ b/Baseline_summary.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinak\PyCharmsProjects\try\CV_Project-Splatter_Image\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5290103C-236E-49A7-91CB-39F9FCF0B027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0BEF5D-1201-458E-811E-3F45F77DAD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{511D045E-1463-4C14-85B5-DFD0A019755E}"/>
+    <workbookView xWindow="348" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{511D045E-1463-4C14-85B5-DFD0A019755E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="srn_cars_100%" sheetId="4" r:id="rId2"/>
-    <sheet name="srn_cars_50%" sheetId="5" r:id="rId3"/>
-    <sheet name="srn_cars_20%" sheetId="6" r:id="rId4"/>
-    <sheet name="co3d_w_background" sheetId="2" r:id="rId5"/>
-    <sheet name="co3d_wo_background" sheetId="7" r:id="rId6"/>
+    <sheet name="srn_cars_100%" sheetId="4" r:id="rId1"/>
+    <sheet name="srn_cars_50%" sheetId="5" r:id="rId2"/>
+    <sheet name="srn_cars_20%" sheetId="6" r:id="rId3"/>
+    <sheet name="co3d_w_background" sheetId="2" r:id="rId4"/>
+    <sheet name="co3d_wo_background" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="42">
   <si>
     <t>model3</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>RGBD_NN</t>
-  </si>
-  <si>
-    <t>RGBD_NN_OUT_DEPTH</t>
   </si>
   <si>
     <t>cars_co3d with background</t>
@@ -581,6 +578,1328 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B34FC15-96D8-4303-9AB1-880B3B105DEB}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-1.9666697677095</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-1.92777</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-1.9505999999999999</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-1.89552819209829</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-1.86063</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-1.88059</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.69253510035399302</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-0.67934000000000005</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-0.68359999999999999</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>24.5525351522321</v>
+      </c>
+      <c r="C16" s="1">
+        <v>24.716734161431098</v>
+      </c>
+      <c r="D16" s="1">
+        <v>24.389944022352001</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.93258934129368098</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.93650351981209001</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.93189543384042595</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.15133590520020901</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.15061360494953299</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.155842035871253</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="7">
+        <v>19.556921948736299</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18.931579110131299</v>
+      </c>
+      <c r="D19" s="1">
+        <v>19.4644615606726</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.83340076460011903</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.824433115605264</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.83611995374411197</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.25596143542445998</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.26398986027508298</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.25300177754326297</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>40</v>
+      </c>
+      <c r="C23" s="1">
+        <v>46</v>
+      </c>
+      <c r="D23" s="1">
+        <v>60</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1">
+        <v>36</v>
+      </c>
+      <c r="D24" s="1">
+        <v>39</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72949DC4-D34C-4434-B271-9E5CE6E9CA21}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-1.9105099999999999</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-1.99211</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-2.0394600000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-1.84348</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-1.91327</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-1.9544600000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.66279999999999994</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-0.67184999999999995</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-0.68501999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>24.843500100753499</v>
+      </c>
+      <c r="C16" s="1">
+        <v>24.776949598030601</v>
+      </c>
+      <c r="D16" s="1">
+        <v>24.568996774879299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.93690909885547302</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.93665950592945901</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.93394670195200202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.14556497367183499</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.14911564117805501</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.15085613816468499</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6">
+        <v>19.529018503075299</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18.974213619055998</v>
+      </c>
+      <c r="D19" s="1">
+        <v>19.4829776251654</v>
+      </c>
+      <c r="G19">
+        <f>MAX(B19:F19)</f>
+        <v>19.529018503075299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.83261579134111996</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.82252721977640197</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.83742460306056499</v>
+      </c>
+      <c r="G20">
+        <f>MAX(B20:F20)</f>
+        <v>0.83742460306056499</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.25399046462350899</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.26509950286700301</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.249459170793945</v>
+      </c>
+      <c r="G21">
+        <f>MIN(B21:F21)</f>
+        <v>0.249459170793945</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>30</v>
+      </c>
+      <c r="C23" s="1">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1">
+        <v>26</v>
+      </c>
+      <c r="D24" s="1">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B20978-D809-4F22-B392-B7FE2B5D1F45}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-2.0167199999999998</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-1.96295</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-1.97624</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-1.67428</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-1.93493</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-1.8900699999999999</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-1.90368</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-1.61931</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.67979999999999996</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-0.67803999999999998</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-0.69328999999999996</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-0.51312999999999998</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>24.595531480652902</v>
+      </c>
+      <c r="C16" s="1">
+        <v>24.678975658757299</v>
+      </c>
+      <c r="D16" s="1">
+        <v>24.4577316045761</v>
+      </c>
+      <c r="E16" s="1">
+        <v>14.9439022881644</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.93330415189266203</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.93395875309194798</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.93258147111960799</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.73801240793296197</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.15459601692855299</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.154813281074166</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.153533073301826</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.32750347650476802</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>19.308173245702399</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18.725503152489601</v>
+      </c>
+      <c r="D19" s="6">
+        <v>19.317035862513901</v>
+      </c>
+      <c r="E19" s="1">
+        <v>13.3197594721317</v>
+      </c>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.82982315452780098</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.81939109509672403</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.83297753747871905</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.64797816423518295</v>
+      </c>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.25545847610831202</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.26631626155525401</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.25675172067241903</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.39727669408959898</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1">
+        <v>61</v>
+      </c>
+      <c r="D23" s="1">
+        <v>26</v>
+      </c>
+      <c r="E23" s="1">
+        <v>60</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1">
+        <v>35</v>
+      </c>
+      <c r="D24" s="1">
+        <v>18</v>
+      </c>
+      <c r="E24" s="1">
+        <v>36</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87F2600-C40F-4D16-A365-57F60FE41D1F}">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>128</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>64</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20000</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-1.45949</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-1.36934</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-1.39194</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-1.3091600000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.20835000000000001</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-0.16894999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>22.1906239986419</v>
+      </c>
+      <c r="C16" s="1">
+        <v>21.0609602332115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.71046415865421297</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.64678486585617001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.39445140957832298</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.48273735195398298</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6">
+        <v>14.001488065138</v>
+      </c>
+      <c r="C19" s="1">
+        <v>13.9242058409802</v>
+      </c>
+      <c r="I19">
+        <f>MAX(B19:C19)</f>
+        <v>14.001488065138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.38057947905823297</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.37298560538075598</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ref="I20" si="0">MAX(B20:C20)</f>
+        <v>0.38057947905823297</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.67616527564101303</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.68830526059604002</v>
+      </c>
+      <c r="I21">
+        <f>MIN(B21:C21)</f>
+        <v>0.67616527564101303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>157</v>
+      </c>
+      <c r="C23" s="1">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FC7724-FE73-4AF6-9A61-4A0445399B4C}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>-1.4845600000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-1.4308799999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>-0.33359</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>27.3742079734802</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.92927645742893195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.13171484395861599</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>16.589788734894899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.54950548779116803</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.42677373654784101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCB9662-65BF-4657-A953-9C7BF6383DF1}">
   <dimension ref="A1:M99"/>
   <sheetViews>
@@ -2127,1341 +3446,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B34FC15-96D8-4303-9AB1-880B3B105DEB}">
-  <dimension ref="A1:F24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1">
-        <v>-1.9666697677095</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-1.92777</v>
-      </c>
-      <c r="D12" s="1">
-        <v>-1.9505999999999999</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1">
-        <v>-1.89552819209829</v>
-      </c>
-      <c r="C13" s="1">
-        <v>-1.86063</v>
-      </c>
-      <c r="D13" s="1">
-        <v>-1.88059</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1">
-        <v>-0.69253510035399302</v>
-      </c>
-      <c r="C14" s="1">
-        <v>-0.67934000000000005</v>
-      </c>
-      <c r="D14" s="1">
-        <v>-0.68359999999999999</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1">
-        <v>24.5525351522321</v>
-      </c>
-      <c r="C16" s="1">
-        <v>24.716734161431098</v>
-      </c>
-      <c r="D16" s="1">
-        <v>24.389944022352001</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0.93258934129368098</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.93650351981209001</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0.93189543384042595</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.15133590520020901</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.15061360494953299</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.155842035871253</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="7">
-        <v>19.556921948736299</v>
-      </c>
-      <c r="C19" s="1">
-        <v>18.931579110131299</v>
-      </c>
-      <c r="D19" s="1">
-        <v>19.4644615606726</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.83340076460011903</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0.824433115605264</v>
-      </c>
-      <c r="D20" s="7">
-        <v>0.83611995374411197</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.25596143542445998</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.26398986027508298</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0.25300177754326297</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1">
-        <v>40</v>
-      </c>
-      <c r="C23" s="1">
-        <v>46</v>
-      </c>
-      <c r="D23" s="1">
-        <v>60</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1">
-        <v>30</v>
-      </c>
-      <c r="C24" s="1">
-        <v>36</v>
-      </c>
-      <c r="D24" s="1">
-        <v>39</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72949DC4-D34C-4434-B271-9E5CE6E9CA21}">
-  <dimension ref="A1:G24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1">
-        <v>-1.9105099999999999</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-1.99211</v>
-      </c>
-      <c r="D12" s="1">
-        <v>-2.0394600000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1">
-        <v>-1.84348</v>
-      </c>
-      <c r="C13" s="1">
-        <v>-1.91327</v>
-      </c>
-      <c r="D13" s="1">
-        <v>-1.9544600000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1">
-        <v>-0.66279999999999994</v>
-      </c>
-      <c r="C14" s="1">
-        <v>-0.67184999999999995</v>
-      </c>
-      <c r="D14" s="1">
-        <v>-0.68501999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1">
-        <v>24.843500100753499</v>
-      </c>
-      <c r="C16" s="1">
-        <v>24.776949598030601</v>
-      </c>
-      <c r="D16" s="1">
-        <v>24.568996774879299</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0.93690909885547302</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.93665950592945901</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0.93394670195200202</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.14556497367183499</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.14911564117805501</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.15085613816468499</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="6">
-        <v>19.529018503075299</v>
-      </c>
-      <c r="C19" s="1">
-        <v>18.974213619055998</v>
-      </c>
-      <c r="D19" s="1">
-        <v>19.4829776251654</v>
-      </c>
-      <c r="G19">
-        <f>MAX(B19:F19)</f>
-        <v>19.529018503075299</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.83261579134111996</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0.82252721977640197</v>
-      </c>
-      <c r="D20" s="6">
-        <v>0.83742460306056499</v>
-      </c>
-      <c r="G20">
-        <f>MAX(B20:F20)</f>
-        <v>0.83742460306056499</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.25399046462350899</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.26509950286700301</v>
-      </c>
-      <c r="D21" s="6">
-        <v>0.249459170793945</v>
-      </c>
-      <c r="G21">
-        <f>MIN(B21:F21)</f>
-        <v>0.249459170793945</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1">
-        <v>30</v>
-      </c>
-      <c r="C23" s="1">
-        <v>36</v>
-      </c>
-      <c r="D23" s="1">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1">
-        <v>23</v>
-      </c>
-      <c r="C24" s="1">
-        <v>26</v>
-      </c>
-      <c r="D24" s="1">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B20978-D809-4F22-B392-B7FE2B5D1F45}">
-  <dimension ref="A1:F24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="22.09765625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1">
-        <v>-2.0167199999999998</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-1.96295</v>
-      </c>
-      <c r="D12" s="1">
-        <v>-1.97624</v>
-      </c>
-      <c r="E12" s="1">
-        <v>-1.67428</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1">
-        <v>-1.93493</v>
-      </c>
-      <c r="C13" s="1">
-        <v>-1.8900699999999999</v>
-      </c>
-      <c r="D13" s="1">
-        <v>-1.90368</v>
-      </c>
-      <c r="E13" s="1">
-        <v>-1.61931</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1">
-        <v>-0.67979999999999996</v>
-      </c>
-      <c r="C14" s="1">
-        <v>-0.67803999999999998</v>
-      </c>
-      <c r="D14" s="1">
-        <v>-0.69328999999999996</v>
-      </c>
-      <c r="E14" s="1">
-        <v>-0.51312999999999998</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1">
-        <v>24.595531480652902</v>
-      </c>
-      <c r="C16" s="1">
-        <v>24.678975658757299</v>
-      </c>
-      <c r="D16" s="1">
-        <v>24.4577316045761</v>
-      </c>
-      <c r="E16" s="1">
-        <v>14.9439022881644</v>
-      </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0.93330415189266203</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.93395875309194798</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0.93258147111960799</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0.73801240793296197</v>
-      </c>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.15459601692855299</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.154813281074166</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.153533073301826</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0.32750347650476802</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="1">
-        <v>19.308173245702399</v>
-      </c>
-      <c r="C19" s="1">
-        <v>18.725503152489601</v>
-      </c>
-      <c r="D19" s="6">
-        <v>19.317035862513901</v>
-      </c>
-      <c r="E19" s="1">
-        <v>13.3197594721317</v>
-      </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.82982315452780098</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0.81939109509672403</v>
-      </c>
-      <c r="D20" s="6">
-        <v>0.83297753747871905</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0.64797816423518295</v>
-      </c>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="6">
-        <v>0.25545847610831202</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.26631626155525401</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0.25675172067241903</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0.39727669408959898</v>
-      </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1">
-        <v>25</v>
-      </c>
-      <c r="C23" s="1">
-        <v>61</v>
-      </c>
-      <c r="D23" s="1">
-        <v>26</v>
-      </c>
-      <c r="E23" s="1">
-        <v>60</v>
-      </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1">
-        <v>18</v>
-      </c>
-      <c r="C24" s="1">
-        <v>35</v>
-      </c>
-      <c r="D24" s="1">
-        <v>18</v>
-      </c>
-      <c r="E24" s="1">
-        <v>36</v>
-      </c>
-      <c r="F24" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87F2600-C40F-4D16-A365-57F60FE41D1F}">
-  <dimension ref="A1:I27"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.09765625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>128</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>64</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>20000</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2000</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1">
-        <v>-1.45949</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-1.36934</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1">
-        <v>-1.39194</v>
-      </c>
-      <c r="C13" s="1">
-        <v>-1.3091600000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1">
-        <v>-0.20835000000000001</v>
-      </c>
-      <c r="C14" s="1">
-        <v>-0.16894999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1">
-        <v>22.1906239986419</v>
-      </c>
-      <c r="C16" s="1">
-        <v>21.0609602332115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0.71046415865421297</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.64678486585617001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.39445140957832298</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.48273735195398298</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="6">
-        <v>14.001488065138</v>
-      </c>
-      <c r="C19" s="1">
-        <v>13.9242058409802</v>
-      </c>
-      <c r="I19">
-        <f>MAX(B19:C19)</f>
-        <v>14.001488065138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="6">
-        <v>0.38057947905823297</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0.37298560538075598</v>
-      </c>
-      <c r="I20">
-        <f t="shared" ref="I20" si="0">MAX(B20:C20)</f>
-        <v>0.38057947905823297</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="6">
-        <v>0.67616527564101303</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.68830526059604002</v>
-      </c>
-      <c r="I21">
-        <f>MIN(B21:C21)</f>
-        <v>0.67616527564101303</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1">
-        <v>157</v>
-      </c>
-      <c r="C23" s="1">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1">
-        <v>22</v>
-      </c>
-      <c r="C24" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43FC7724-FE73-4AF6-9A61-4A0445399B4C}">
-  <dimension ref="A1:C27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.19921875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1">
-        <v>-1.4845600000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1">
-        <v>-1.4308799999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1">
-        <v>-0.33359</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1">
-        <v>27.3742079734802</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0.92927645742893195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.13171484395861599</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="1">
-        <v>16.589788734894899</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.54950548779116803</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.42677373654784101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>